<commit_message>
Making a bit more generic.
</commit_message>
<xml_diff>
--- a/resources/sparse-sample.xlsx
+++ b/resources/sparse-sample.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
-  <si>
-    <t xml:space="preserve">Node ID</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+  <si>
+    <t xml:space="preserve">Item</t>
   </si>
   <si>
     <t xml:space="preserve">Set</t>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">Quickdraw Morrocco</t>
   </si>
   <si>
-    <t xml:space="preserve">Batman Robin</t>
+    <t xml:space="preserve">Batman</t>
   </si>
   <si>
     <t xml:space="preserve">Capacity</t>
@@ -70,28 +70,34 @@
     <t xml:space="preserve">Field</t>
   </si>
   <si>
-    <t xml:space="preserve">QD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pc_rand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pc_read</t>
-  </si>
-  <si>
-    <t xml:space="preserve">qos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jira</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes</t>
+    <t xml:space="preserve">Hello</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yeah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Its</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Been</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A_While</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Much</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How</t>
+  </si>
+  <si>
+    <t xml:space="preserve">About</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You</t>
   </si>
   <si>
     <t xml:space="preserve">Something</t>
@@ -208,8 +214,8 @@
   </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="34:34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -218,7 +224,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.58"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
@@ -229,10 +235,10 @@
         <v>0</v>
       </c>
       <c r="G1" s="0" t="n">
-        <v>90001</v>
+        <v>111000</v>
       </c>
       <c r="H1" s="0" t="n">
-        <v>90001</v>
+        <v>111000</v>
       </c>
       <c r="I1" s="0" t="n">
         <v>123456</v>
@@ -331,18 +337,18 @@
         <v>22</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -362,19 +368,19 @@
         <v>0</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>546</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>789</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K11" s="0" t="n">
         <v>10</v>
@@ -397,7 +403,7 @@
         <v>70</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G12" s="0" t="n">
         <v>123</v>
@@ -406,7 +412,7 @@
         <v>234</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="K12" s="0" t="n">
         <v>20</v>

</xml_diff>